<commit_message>
Fixed formula cells for Lon and Lat
Added the formula used to calculate Lat and Lon in decimal degrees.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL376_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL376_00003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leila/Documents/OOI_assmgt/asset-management/deployment/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="3080" windowWidth="23460" windowHeight="10240" tabRatio="377"/>
+    <workbookView xWindow="49920" yWindow="680" windowWidth="23460" windowHeight="10240" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -32,6 +37,9 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -364,10 +372,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -476,7 +494,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -491,6 +509,11 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -505,6 +528,11 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 15" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -877,13 +905,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -894,7 +922,7 @@
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28">
+    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>37</v>
       </c>
@@ -932,7 +960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="25" customFormat="1" ht="15">
+    <row r="2" spans="1:14" s="25" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -969,63 +997,66 @@
       <c r="L2" s="26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="25">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
+        <v>39.833333333333336</v>
+      </c>
+      <c r="N2" s="25">
+        <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
+        <v>-70.708333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1037,7 +1068,7 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -1049,7 +1080,7 @@
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28">
+    <row r="1" spans="1:19" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
@@ -1114,7 +1145,7 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1153,7 +1184,7 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1192,7 +1223,7 @@
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -1231,7 +1262,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="9"/>
@@ -1252,7 +1283,7 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1286,7 +1317,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:19" s="2" customFormat="1">
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1320,7 +1351,7 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1">
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1385,7 @@
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:19" s="2" customFormat="1">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1388,7 +1419,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:19" s="2" customFormat="1">
+    <row r="11" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="9"/>
@@ -1404,7 +1435,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:19" s="2" customFormat="1">
+    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -1434,7 +1465,7 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:19" s="2" customFormat="1">
+    <row r="13" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="9"/>
@@ -1450,7 +1481,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:19" s="2" customFormat="1">
+    <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1480,7 +1511,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:19" s="2" customFormat="1">
+    <row r="15" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="9"/>
@@ -1496,7 +1527,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:19" s="2" customFormat="1">
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
@@ -1528,7 +1559,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="9"/>
@@ -1544,7 +1575,7 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
@@ -1574,7 +1605,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:14" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -1590,13 +1621,13 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1605,10 +1636,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>